<commit_message>
Updated spelling of Ringgold
</commit_message>
<xml_diff>
--- a/xlsx/organisation-identifier-type.xlsx
+++ b/xlsx/organisation-identifier-type.xlsx
@@ -71,10 +71,10 @@
     <t xml:space="preserve">06</t>
   </si>
   <si>
-    <t xml:space="preserve">Ringold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ringold identifier for organisations in the publishing industry supply chain</t>
+    <t xml:space="preserve">Ringgold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ringgold identifier for organisations in the publishing industry supply chain</t>
   </si>
   <si>
     <t xml:space="preserve">07</t>

</xml_diff>

<commit_message>
Updated Organisation Identifier Type to include EDUMIS number
</commit_message>
<xml_diff>
--- a/xlsx/organisation-identifier-type.xlsx
+++ b/xlsx/organisation-identifier-type.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t xml:space="preserve">Global Research Identifier Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUMIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier for educational providers registered with the Ministry of Education's Education Management Information System (EDUMIS)</t>
   </si>
   <si>
     <t xml:space="preserve">99</t>
@@ -579,6 +588,20 @@
         <v>31</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>